<commit_message>
ListMaker Price 계산 수정
</commit_message>
<xml_diff>
--- a/EdiUtils/Resources/template_850_List2.xlsx
+++ b/EdiUtils/Resources/template_850_List2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deHong\source\repos\EdiUtils\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deHong\source\repos\FBH-EDI-Utils\EdiUtils\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F78655A-0110-40EE-8EF1-5F1866718506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A41DFF7-D058-4700-910E-27DF14EB0893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="27825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30137" yWindow="574" windowWidth="28817" windowHeight="10937" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listing PO" sheetId="2" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>SSCC-18 Number</t>
   </si>
   <si>
-    <t>Tracking Number</t>
-  </si>
-  <si>
     <t>Shipping Id</t>
   </si>
   <si>
@@ -192,6 +189,10 @@
   </si>
   <si>
     <t>Oreder Amount</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit Price</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -203,7 +204,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,30 +523,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -566,6 +543,30 @@
     </xf>
     <xf numFmtId="41" fontId="10" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -885,13 +886,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R109" sqref="R109"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.875" style="4" customWidth="1"/>
@@ -902,7 +903,8 @@
     <col min="8" max="8" width="17.375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.375" style="5" customWidth="1"/>
     <col min="10" max="11" width="17.625" style="4" customWidth="1"/>
-    <col min="12" max="14" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="9" style="4" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="4" customWidth="1"/>
     <col min="15" max="15" width="9.125" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.375" style="4" hidden="1" customWidth="1"/>
     <col min="17" max="18" width="0" style="4" hidden="1" customWidth="1"/>
@@ -916,9 +918,9 @@
     <col min="32" max="32" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1">
+    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -930,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -957,48 +959,48 @@
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X1" s="2"/>
       <c r="Y1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="AF1" s="1"/>
     </row>
@@ -1013,227 +1015,227 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB240C3-7C62-4146-9D66-81B50CAB3F8D}">
   <dimension ref="B2:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="14.75" customWidth="1"/>
     <col min="8" max="9" width="13.25" customWidth="1"/>
     <col min="14" max="14" width="13.25" customWidth="1"/>
-    <col min="16" max="16" width="9.375" style="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.375" style="28" customWidth="1"/>
-    <col min="18" max="18" width="15.375" style="29" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9" style="29"/>
-    <col min="21" max="21" width="9" style="28"/>
-    <col min="22" max="22" width="15.375" style="29" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.875" style="29" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.875" style="28" customWidth="1"/>
-    <col min="26" max="26" width="15.375" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.375" style="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.375" style="20" customWidth="1"/>
+    <col min="18" max="18" width="15.375" style="21" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" style="21"/>
+    <col min="21" max="21" width="9" style="20"/>
+    <col min="22" max="22" width="15.375" style="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.875" style="21" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.875" style="20" customWidth="1"/>
+    <col min="26" max="26" width="15.375" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B2" s="24" t="s">
+    <row r="2" spans="2:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
+      <c r="P2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="16"/>
+      <c r="T2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="23"/>
-      <c r="P2" s="26" t="s">
+      <c r="U2" s="22"/>
+      <c r="V2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26" t="s">
+      <c r="W2" s="16"/>
+      <c r="X2" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" s="16"/>
-      <c r="X2" s="30" t="s">
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="32"/>
+      <c r="C3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="2:26" ht="17.25" thickBot="1">
-      <c r="B3" s="25"/>
-      <c r="C3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="32">
+      <c r="Q3" s="18"/>
+      <c r="R3" s="24">
         <f>SUM(R5:R46)</f>
         <v>0</v>
       </c>
       <c r="S3" s="16"/>
-      <c r="T3" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="U3" s="30"/>
-      <c r="V3" s="32">
+      <c r="T3" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="22"/>
+      <c r="V3" s="24">
         <f>SUM(V5:V21)</f>
         <v>0</v>
       </c>
       <c r="W3" s="16"/>
-      <c r="X3" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y3" s="30"/>
-      <c r="Z3" s="32">
+      <c r="X3" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="24">
         <f>SUM(Z5:Z24)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:26" ht="17.25" thickBot="1">
-      <c r="B4" s="18" t="s">
+    <row r="4" spans="2:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="12"/>
-      <c r="I4" s="20"/>
+      <c r="I4" s="27"/>
       <c r="J4" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
       <c r="N4" s="12"/>
-      <c r="P4" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27" t="s">
-        <v>42</v>
+      <c r="P4" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="S4" s="16"/>
-      <c r="T4" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27" t="s">
-        <v>42</v>
+      <c r="T4" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="W4" s="16"/>
-      <c r="X4" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" s="31"/>
-      <c r="Z4" s="31" t="s">
-        <v>42</v>
+      <c r="X4" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:26">
-      <c r="B5" s="19"/>
-      <c r="C5" s="21"/>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B5" s="26"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="21"/>
+      <c r="I5" s="28"/>
       <c r="J5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
-      <c r="P5" s="28"/>
-      <c r="R5" s="28"/>
+      <c r="P5" s="20"/>
+      <c r="R5" s="20"/>
       <c r="S5" s="17"/>
-      <c r="T5" s="28"/>
-      <c r="V5" s="28"/>
+      <c r="T5" s="20"/>
+      <c r="V5" s="20"/>
       <c r="W5" s="17"/>
-      <c r="X5" s="28"/>
-      <c r="Z5" s="28"/>
+      <c r="X5" s="20"/>
+      <c r="Z5" s="20"/>
     </row>
-    <row r="6" spans="2:26">
-      <c r="P6" s="28"/>
-      <c r="R6" s="28"/>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="P6" s="20"/>
+      <c r="R6" s="20"/>
       <c r="S6" s="17"/>
-      <c r="T6" s="28"/>
-      <c r="V6" s="28"/>
+      <c r="T6" s="20"/>
+      <c r="V6" s="20"/>
       <c r="W6" s="17"/>
-      <c r="X6" s="28"/>
-      <c r="Z6" s="28"/>
+      <c r="X6" s="20"/>
+      <c r="Z6" s="20"/>
     </row>
-    <row r="7" spans="2:26">
-      <c r="P7" s="28"/>
-      <c r="R7" s="28"/>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="P7" s="20"/>
+      <c r="R7" s="20"/>
       <c r="S7" s="17"/>
-      <c r="T7" s="28"/>
-      <c r="V7" s="28"/>
+      <c r="T7" s="20"/>
+      <c r="V7" s="20"/>
       <c r="W7" s="17"/>
-      <c r="X7" s="28"/>
-      <c r="Z7" s="28"/>
+      <c r="X7" s="20"/>
+      <c r="Z7" s="20"/>
     </row>
-    <row r="20" spans="9:9">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I20" s="9"/>
     </row>
   </sheetData>

</xml_diff>